<commit_message>
Add new M3 hole entry
</commit_message>
<xml_diff>
--- a/hardware/Printed Hole Size Dictionary.xlsx
+++ b/hardware/Printed Hole Size Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubRepos\OhPossum-hw\OhPossum\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803860D1-7909-4A0A-814B-823978B25A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A081D125-873F-4031-8B69-3E107860C7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD663A06-41EE-4F1E-90FA-5F3970629C54}"/>
   </bookViews>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,19 +1712,19 @@
         <v>36</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M8" si="3">(L3+0.2926) / 0.9917</f>
+        <f t="shared" ref="M3:M9" si="3">(L3+0.2926) / 0.9917</f>
         <v>36.596349702531008</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N8" si="4">L3+H3</f>
+        <f t="shared" ref="N3:N9" si="4">L3+H3</f>
         <v>36.5</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O8" si="5">ROUND(MAX(M3:N3), 1)</f>
+        <f t="shared" ref="O3:O9" si="5">ROUND(MAX(M3:N3), 1)</f>
         <v>36.6</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P8" si="6">O3/2</f>
+        <f t="shared" ref="P3:P9" si="6">O3/2</f>
         <v>18.3</v>
       </c>
     </row>
@@ -1983,6 +1983,25 @@
       <c r="H9">
         <f t="shared" si="2"/>
         <v>0.39500000000000002</v>
+      </c>
+      <c r="L9">
+        <v>2.9</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>3.2193203589795303</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>3.2949999999999999</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>3.3</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>1.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new M3 threaded insert and encoder magnet hole entries
</commit_message>
<xml_diff>
--- a/hardware/Printed Hole Size Dictionary.xlsx
+++ b/hardware/Printed Hole Size Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubRepos\OhPossum-hw\OhPossum\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A081D125-873F-4031-8B69-3E107860C7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F517257D-2460-4B01-A480-05C039CDEC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD663A06-41EE-4F1E-90FA-5F3970629C54}"/>
   </bookViews>
@@ -1577,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE5CB1F-97D2-4B1B-9D30-732217DA17D4}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,19 +1712,19 @@
         <v>36</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M9" si="3">(L3+0.2926) / 0.9917</f>
+        <f t="shared" ref="M3:M11" si="3">(L3+0.2926) / 0.9917</f>
         <v>36.596349702531008</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N9" si="4">L3+H3</f>
+        <f t="shared" ref="N3:N11" si="4">L3+H3</f>
         <v>36.5</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O9" si="5">ROUND(MAX(M3:N3), 1)</f>
+        <f t="shared" ref="O3:O11" si="5">ROUND(MAX(M3:N3), 1)</f>
         <v>36.6</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P9" si="6">O3/2</f>
+        <f t="shared" ref="P3:P11" si="6">O3/2</f>
         <v>18.3</v>
       </c>
     </row>
@@ -2002,6 +2002,48 @@
       <c r="P9">
         <f t="shared" si="6"/>
         <v>1.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>4.7318745588383591</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>4.7</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>8.3620046384995455</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>8.4</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>4.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>